<commit_message>
0904 1312 F10 -> git, reorganize
</commit_message>
<xml_diff>
--- a/Note/Plan for F key.xlsx
+++ b/Note/Plan for F key.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Plan for MTK" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>Key</t>
   </si>
@@ -247,24 +247,12 @@
     <t>Add image by customer request</t>
   </si>
   <si>
-    <t xml:space="preserve">Set makefile </t>
-  </si>
-  <si>
-    <t>Set makefile current</t>
-  </si>
-  <si>
     <t>Open version info (make\Verno_(PROJECT).bld)</t>
   </si>
   <si>
     <t>Quickly change verno</t>
   </si>
   <si>
-    <t>Open build folder</t>
-  </si>
-  <si>
-    <t>Open current build folder</t>
-  </si>
-  <si>
     <r>
       <t>Project-specific files (</t>
     </r>
@@ -306,12 +294,6 @@
     <t xml:space="preserve">Custom </t>
   </si>
   <si>
-    <t>PlutoMMI</t>
-  </si>
-  <si>
-    <t>Open MMI (plutommi)</t>
-  </si>
-  <si>
     <t>Debugging</t>
   </si>
   <si>
@@ -321,15 +303,6 @@
     <t>Edit chglog of build</t>
   </si>
   <si>
-    <t>Catcher</t>
-  </si>
-  <si>
-    <t>FlashTool</t>
-  </si>
-  <si>
-    <t>MoDIS</t>
-  </si>
-  <si>
     <t>Quickly test UI/feature changes pre-real device</t>
   </si>
   <si>
@@ -489,6 +462,69 @@
     <t>Change menuitem</t>
   </si>
   <si>
+    <t>Open driver folder (MS_Customize\source\product\driver)</t>
+  </si>
+  <si>
+    <t>Open custom folder (MS_Customize\source\product\config\fp6531_bar)</t>
+  </si>
+  <si>
+    <t>MMI</t>
+  </si>
+  <si>
+    <t>Open MMI (MS_MMI\source)</t>
+  </si>
+  <si>
+    <t>ArmLogel</t>
+  </si>
+  <si>
+    <t>ResearchDownload</t>
+  </si>
+  <si>
+    <t>Simulator</t>
+  </si>
+  <si>
+    <t>Open nveditor</t>
+  </si>
+  <si>
+    <t>Change NV item</t>
+  </si>
+  <si>
+    <t>Set Default makefile</t>
+  </si>
+  <si>
+    <t>Set default project</t>
+  </si>
+  <si>
+    <t>Open project data folder</t>
+  </si>
+  <si>
+    <t>Project Info (details: flash,lcd,spkr,pbook)</t>
+  </si>
+  <si>
+    <t>Search backwards</t>
+  </si>
+  <si>
+    <t>Search forwards</t>
+  </si>
+  <si>
+    <t>Commit to Git: RZ BWV3 -&gt; game mode key</t>
+  </si>
+  <si>
+    <t>Project Info: RZ BWV3 -&gt; macro mode key</t>
+  </si>
+  <si>
+    <t>Compare by WinMerge / BeyondCompare</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Debug (real device)</t>
+  </si>
+  <si>
+    <t>Redmine</t>
+  </si>
+  <si>
     <r>
       <t>Open audiores folder (</t>
     </r>
@@ -501,7 +537,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>I:\project_SPD\SC6531DA\MS_MMI\source\resource\(PROJECT)\RING</t>
+      <t>MS_MMI\source\resource\(PROJECT)\RING</t>
     </r>
     <r>
       <rPr>
@@ -527,7 +563,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>I:\project_SPD\SC6531DA\MS_MMI\source\resource\(PROJECT)\IMAG</t>
+      <t>MS_MMI\source\resource\(PROJECT)\IMAG</t>
     </r>
     <r>
       <rPr>
@@ -539,33 +575,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>Open driver folder (MS_Customize\source\product\driver)</t>
-  </si>
-  <si>
-    <t>Open custom folder (MS_Customize\source\product\config\fp6531_bar)</t>
-  </si>
-  <si>
-    <t>MMI</t>
-  </si>
-  <si>
-    <t>Open MMI (MS_MMI\source)</t>
-  </si>
-  <si>
-    <t>ArmLogel</t>
-  </si>
-  <si>
-    <t>ResearchDownload</t>
-  </si>
-  <si>
-    <t>Simulator</t>
-  </si>
-  <si>
-    <t>Open nveditor</t>
-  </si>
-  <si>
-    <t>Change NV item</t>
   </si>
 </sst>
 </file>
@@ -615,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -637,6 +646,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -964,15 +982,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1002,7 +1020,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -1041,125 +1059,125 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>65</v>
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
+      <c r="B14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
+      <c r="B16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,10 +1185,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,11 +1196,56 @@
         <v>14</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1192,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1232,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -1243,10 +1306,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1254,10 +1317,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1265,10 +1328,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1276,35 +1339,35 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1312,128 +1375,128 @@
         <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,10 +1504,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,10 +1515,87 @@
         <v>14</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0904 1511 help (git help as starter), string from escape
</commit_message>
<xml_diff>
--- a/Note/Plan for F key.xlsx
+++ b/Note/Plan for F key.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="10245" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan for MTK" sheetId="1" r:id="rId1"/>
     <sheet name="Plan for SPRD" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan for Base" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="96">
   <si>
     <t>Key</t>
   </si>
@@ -522,9 +523,6 @@
     <t>Debug (real device)</t>
   </si>
   <si>
-    <t>Redmine</t>
-  </si>
-  <si>
     <r>
       <t>Open audiores folder (</t>
     </r>
@@ -575,6 +573,36 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Write reason in wip</t>
+  </si>
+  <si>
+    <t>Open macros folder</t>
+  </si>
+  <si>
+    <t>Open config folder</t>
+  </si>
+  <si>
+    <t>Open notes folder</t>
+  </si>
+  <si>
+    <t>Goto</t>
+  </si>
+  <si>
+    <t>Open personal folder</t>
+  </si>
+  <si>
+    <t>Open personal note folder</t>
+  </si>
+  <si>
+    <t>Create macro body</t>
+  </si>
+  <si>
+    <t>Put next pressed key to file</t>
   </si>
 </sst>
 </file>
@@ -938,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="A16:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,26 +1142,26 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,10 +1169,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1258,7 +1286,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C19" sqref="A16:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,7 +1378,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>27</v>
@@ -1361,7 +1389,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>34</v>
@@ -1433,26 +1461,26 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,10 +1488,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1597,6 +1625,325 @@
       <c r="C45" s="2" t="s">
         <v>51</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>